<commit_message>
11a - analyza pc pre sikmy tah
</commit_message>
<xml_diff>
--- a/nim/analyzaPC.xlsx
+++ b/nim/analyzaPC.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\inf\2021\5ZYI11\nim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DBE5F56-8E09-4651-82C4-ABD2066CE5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5C3C15-5F8F-4585-AFC3-5AACFE453DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27405" yWindow="5040" windowWidth="20760" windowHeight="15435" xr2:uid="{26BC7A31-AC86-48FF-92A4-926A9367963B}"/>
+    <workbookView xWindow="-27405" yWindow="5040" windowWidth="20760" windowHeight="15435" activeTab="2" xr2:uid="{26BC7A31-AC86-48FF-92A4-926A9367963B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
+    <sheet name="bezSikmehoTahu" sheetId="2" r:id="rId2"/>
+    <sheet name="soSikmymTahom" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -222,6 +230,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -538,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6A661D-0E41-4B17-9BB9-E49DA1BE597A}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,4 +743,218 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63775CF1-CE85-4E00-BA34-ED169117AEB1}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972C7189-BCAF-4D39-9EF4-CBB739C49ACC}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>